<commit_message>
feat: add new row to export
</commit_message>
<xml_diff>
--- a/src/infrastructure/web/controllers/order_details.xlsx
+++ b/src/infrastructure/web/controllers/order_details.xlsx
@@ -635,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>11</v>
+        <v>717</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -646,7 +646,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -657,7 +657,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>494</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>591</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>698</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -690,7 +690,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>650</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>12</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>476</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -734,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>410</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -745,7 +745,7 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>499</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>15</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>871</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>898</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>21</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>22</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>777</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,7 +833,7 @@
         <v>23</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>712</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
         <v>24</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -866,7 +866,7 @@
         <v>26</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
         <v>27</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>571</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -888,7 +888,7 @@
         <v>28</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>717</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>29</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
         <v>30</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>989</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>31</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>227</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>32</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>549</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>33</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,7 +954,7 @@
         <v>34</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>729</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -965,7 +965,7 @@
         <v>35</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,7 +976,7 @@
         <v>36</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>928</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,7 +987,7 @@
         <v>37</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
         <v>38</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>401</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>39</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>911</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>40</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>781</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1031,7 +1031,7 @@
         <v>41</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>774</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>42</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>905</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>43</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>231</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1064,7 +1064,7 @@
         <v>44</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>45</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>46</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>47</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>744</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
         <v>48</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,7 +1119,7 @@
         <v>49</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>672</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,7 +1130,7 @@
         <v>50</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
         <v>51</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>52</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>53</v>
       </c>
       <c r="C50">
-        <v>1</v>
+        <v>710</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
         <v>54</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,7 +1185,7 @@
         <v>55</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>56</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>700</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,7 +1207,7 @@
         <v>57</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>804</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,7 +1218,7 @@
         <v>58</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1229,7 +1229,7 @@
         <v>59</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>388</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
         <v>60</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>372</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1251,7 +1251,7 @@
         <v>61</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
         <v>62</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>825</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
         <v>63</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>276</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>64</v>
       </c>
       <c r="C61">
-        <v>1</v>
+        <v>793</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1295,7 +1295,7 @@
         <v>65</v>
       </c>
       <c r="C62">
-        <v>1</v>
+        <v>390</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1306,7 +1306,7 @@
         <v>66</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>527</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1317,7 +1317,7 @@
         <v>67</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
         <v>68</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>435</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1339,7 +1339,7 @@
         <v>69</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>370</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>70</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1361,7 +1361,7 @@
         <v>71</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>73</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>397</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: add platform id export order
</commit_message>
<xml_diff>
--- a/src/infrastructure/web/controllers/order_details.xlsx
+++ b/src/infrastructure/web/controllers/order_details.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="57">
   <si>
     <t>Proveedor</t>
   </si>
@@ -28,72 +28,18 @@
     <t>Finca Funza</t>
   </si>
   <si>
-    <t>Lechuga Batavia</t>
+    <t>Perejil Crespo</t>
   </si>
   <si>
     <t>Bogotá</t>
   </si>
   <si>
-    <t>Lechuga Verde Lisa</t>
-  </si>
-  <si>
-    <t>Lechuga Verde Crespa</t>
-  </si>
-  <si>
-    <t>Lechuga Morada Crespa</t>
-  </si>
-  <si>
-    <t>Lechuga Romana</t>
-  </si>
-  <si>
-    <t>Lechuga Bambi x 3uni Morada</t>
-  </si>
-  <si>
-    <t>Lechuga Bambi x 3uni Combinada</t>
-  </si>
-  <si>
-    <t>Lechuga Bambi x 3uni Verde</t>
-  </si>
-  <si>
-    <t>Rugula Hindú</t>
-  </si>
-  <si>
-    <t>Rugula Inglesa</t>
-  </si>
-  <si>
-    <t>Rábanos</t>
-  </si>
-  <si>
-    <t>Mix Asiática</t>
-  </si>
-  <si>
-    <t>Perejil Crespo</t>
-  </si>
-  <si>
     <t>Perejil Liso</t>
   </si>
   <si>
-    <t>Kale Imperial</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>Amawa</t>
-  </si>
-  <si>
-    <t>Ensalada Mix Baby Naranja</t>
-  </si>
-  <si>
-    <t>Ensalada Mix Baby Morada</t>
-  </si>
-  <si>
-    <t>Ensalada Mix Baby Verde</t>
-  </si>
-  <si>
-    <t>Ensalada Mix Baby Roja</t>
-  </si>
-  <si>
     <t>William</t>
   </si>
   <si>
@@ -230,9 +176,6 @@
   </si>
   <si>
     <t>Verdolaga</t>
-  </si>
-  <si>
-    <t>Hierbas x Kilo</t>
   </si>
   <si>
     <t>Rosales</t>
@@ -615,7 +558,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D52"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="30" customWidth="1"/>
@@ -644,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -658,7 +601,7 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>408</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -666,27 +609,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>317</v>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>461</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -694,13 +637,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -708,13 +651,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>236</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -722,13 +665,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>677</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -736,13 +679,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>492</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -750,13 +693,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>944</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -764,13 +707,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -778,13 +721,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>635</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -792,13 +735,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13">
-        <v>166</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -806,13 +749,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14">
-        <v>376</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -820,13 +763,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -834,13 +777,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>694</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -848,27 +791,27 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18">
-        <v>715</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
@@ -876,13 +819,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
       </c>
       <c r="C19">
-        <v>753</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -890,13 +833,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
       </c>
       <c r="C20">
-        <v>747</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
@@ -904,13 +847,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
         <v>26</v>
       </c>
       <c r="C21">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
@@ -918,27 +861,27 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="C23">
-        <v>757</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -946,13 +889,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
         <v>29</v>
       </c>
       <c r="C24">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>6</v>
@@ -960,13 +903,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="C25">
-        <v>871</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
         <v>6</v>
@@ -974,13 +917,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>31</v>
       </c>
       <c r="C26">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -988,13 +931,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
       </c>
       <c r="C27">
-        <v>880</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -1002,13 +945,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
         <v>33</v>
       </c>
       <c r="C28">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
@@ -1016,13 +959,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
       </c>
       <c r="C29">
-        <v>135</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
         <v>6</v>
@@ -1030,13 +973,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
       </c>
       <c r="C30">
-        <v>724</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
@@ -1044,13 +987,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
         <v>36</v>
       </c>
       <c r="C31">
-        <v>325</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -1058,13 +1001,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
       </c>
       <c r="C32">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -1072,13 +1015,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>38</v>
       </c>
       <c r="C33">
-        <v>403</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
         <v>6</v>
@@ -1086,13 +1029,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
         <v>39</v>
       </c>
       <c r="C34">
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>6</v>
@@ -1100,13 +1043,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
         <v>40</v>
       </c>
       <c r="C35">
-        <v>428</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>6</v>
@@ -1114,13 +1057,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
         <v>41</v>
       </c>
       <c r="C36">
-        <v>883</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -1128,13 +1071,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
         <v>42</v>
       </c>
       <c r="C37">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1142,13 +1085,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
         <v>43</v>
       </c>
       <c r="C38">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="D38" t="s">
         <v>6</v>
@@ -1156,13 +1099,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
         <v>44</v>
       </c>
       <c r="C39">
-        <v>710</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
         <v>6</v>
@@ -1170,13 +1113,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
         <v>45</v>
       </c>
       <c r="C40">
-        <v>821</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
@@ -1184,13 +1127,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
         <v>46</v>
       </c>
       <c r="C41">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
@@ -1198,13 +1141,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
       </c>
       <c r="C42">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
@@ -1212,13 +1155,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
       </c>
       <c r="C43">
-        <v>926</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -1226,13 +1169,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
         <v>49</v>
       </c>
       <c r="C44">
-        <v>362</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -1240,13 +1183,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
         <v>50</v>
       </c>
       <c r="C45">
-        <v>656</v>
+        <v>0</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1254,13 +1197,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
         <v>51</v>
       </c>
       <c r="C46">
-        <v>582</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
@@ -1268,13 +1211,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
         <v>52</v>
       </c>
       <c r="C47">
-        <v>313</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
@@ -1282,13 +1225,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
         <v>53</v>
       </c>
       <c r="C48">
-        <v>981</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -1296,13 +1239,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
         <v>54</v>
       </c>
       <c r="C49">
-        <v>455</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -1310,27 +1253,27 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
-      </c>
-      <c r="C50">
-        <v>210</v>
+        <v>8</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
         <v>56</v>
       </c>
       <c r="C51">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
@@ -1338,282 +1281,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52">
-        <v>208</v>
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>27</v>
-      </c>
-      <c r="B53" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53">
-        <v>446</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>27</v>
-      </c>
-      <c r="B54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54">
-        <v>193</v>
-      </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>27</v>
-      </c>
-      <c r="B55" t="s">
-        <v>60</v>
-      </c>
-      <c r="C55">
-        <v>391</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>27</v>
-      </c>
-      <c r="B56" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56">
-        <v>919</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>27</v>
-      </c>
-      <c r="B57" t="s">
-        <v>62</v>
-      </c>
-      <c r="C57">
-        <v>512</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>27</v>
-      </c>
-      <c r="B58" t="s">
-        <v>63</v>
-      </c>
-      <c r="C58">
-        <v>437</v>
-      </c>
-      <c r="D58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59">
-        <v>96</v>
-      </c>
-      <c r="D59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B60" t="s">
-        <v>65</v>
-      </c>
-      <c r="C60">
-        <v>982</v>
-      </c>
-      <c r="D60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>27</v>
-      </c>
-      <c r="B61" t="s">
-        <v>66</v>
-      </c>
-      <c r="C61">
-        <v>530</v>
-      </c>
-      <c r="D61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>27</v>
-      </c>
-      <c r="B62" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62">
-        <v>669</v>
-      </c>
-      <c r="D62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>27</v>
-      </c>
-      <c r="B63" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63">
-        <v>691</v>
-      </c>
-      <c r="D63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>27</v>
-      </c>
-      <c r="B64" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64">
-        <v>404</v>
-      </c>
-      <c r="D64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>27</v>
-      </c>
-      <c r="B65" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65">
-        <v>14</v>
-      </c>
-      <c r="D65" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>27</v>
-      </c>
-      <c r="B66" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66">
-        <v>590</v>
-      </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>27</v>
-      </c>
-      <c r="B67" t="s">
-        <v>72</v>
-      </c>
-      <c r="C67">
-        <v>182</v>
-      </c>
-      <c r="D67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>27</v>
-      </c>
-      <c r="B68" t="s">
-        <v>73</v>
-      </c>
-      <c r="C68">
-        <v>805</v>
-      </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>21</v>
-      </c>
-      <c r="B69" t="s">
-        <v>21</v>
-      </c>
-      <c r="C69" t="s">
-        <v>21</v>
-      </c>
-      <c r="D69" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>74</v>
-      </c>
-      <c r="B70" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70">
-        <v>535</v>
-      </c>
-      <c r="D70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>21</v>
-      </c>
-      <c r="B71" t="s">
-        <v>21</v>
-      </c>
-      <c r="C71" t="s">
-        <v>21</v>
-      </c>
-      <c r="D71" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>